<commit_message>
revised all the test code
</commit_message>
<xml_diff>
--- a/RQ1/RQ1_Expanded.xlsx
+++ b/RQ1/RQ1_Expanded.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepak\Documents\MastersDegree\CSI5370-SoftwareVerificationAndTesting\GithubRepos\csi5370project\RQ1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D513936D-0A42-411B-B1A2-18D4FDE79399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FB8E22-9C5E-4082-B937-C40AA5FD67AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="14265" windowWidth="50520" windowHeight="16695" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="555" yWindow="8580" windowWidth="50520" windowHeight="16695" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="8" r:id="rId1"/>
@@ -20151,7 +20151,7 @@
       <pane xSplit="19" ySplit="3" topLeftCell="T4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="T1" sqref="T1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Z50" sqref="Z50"/>
+      <selection pane="bottomRight" activeCell="S53" sqref="S4:W53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -20410,24 +20410,12 @@
       <c r="R4" s="14">
         <v>0</v>
       </c>
-      <c r="S4" s="65">
-        <v>26</v>
-      </c>
-      <c r="T4" s="65">
-        <v>0</v>
-      </c>
-      <c r="U4" s="65">
-        <v>0</v>
-      </c>
-      <c r="V4" s="65">
-        <v>0</v>
-      </c>
-      <c r="W4" s="66">
-        <v>1</v>
-      </c>
-      <c r="X4" s="57">
-        <v>3.6</v>
-      </c>
+      <c r="S4" s="65"/>
+      <c r="T4" s="65"/>
+      <c r="U4" s="65"/>
+      <c r="V4" s="65"/>
+      <c r="W4" s="66"/>
+      <c r="X4" s="57"/>
     </row>
     <row r="5" spans="1:24" ht="95.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="13">
@@ -20484,24 +20472,12 @@
       <c r="R5" s="14">
         <v>4.29</v>
       </c>
-      <c r="S5" s="67">
-        <v>21</v>
-      </c>
-      <c r="T5" s="67">
-        <v>2</v>
-      </c>
-      <c r="U5" s="67">
-        <v>0</v>
-      </c>
-      <c r="V5" s="67">
-        <v>0</v>
-      </c>
-      <c r="W5" s="68">
-        <v>0.9</v>
-      </c>
-      <c r="X5" s="57">
-        <v>1.05</v>
-      </c>
+      <c r="S5" s="67"/>
+      <c r="T5" s="67"/>
+      <c r="U5" s="67"/>
+      <c r="V5" s="67"/>
+      <c r="W5" s="68"/>
+      <c r="X5" s="57"/>
     </row>
     <row r="6" spans="1:24" ht="36.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="13">
@@ -20558,24 +20534,12 @@
       <c r="R6" s="14">
         <v>7.4</v>
       </c>
-      <c r="S6" s="69">
-        <v>13</v>
-      </c>
-      <c r="T6" s="69">
-        <v>12</v>
-      </c>
-      <c r="U6" s="69">
-        <v>4</v>
-      </c>
-      <c r="V6" s="69">
-        <v>0</v>
-      </c>
-      <c r="W6" s="70">
-        <v>0.06</v>
-      </c>
-      <c r="X6" s="57">
-        <v>5.38</v>
-      </c>
+      <c r="S6" s="69"/>
+      <c r="T6" s="69"/>
+      <c r="U6" s="69"/>
+      <c r="V6" s="69"/>
+      <c r="W6" s="70"/>
+      <c r="X6" s="57"/>
     </row>
     <row r="7" spans="1:24" ht="89.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="13">
@@ -20632,24 +20596,12 @@
       <c r="R7" s="14">
         <v>4.74</v>
       </c>
-      <c r="S7" s="67">
-        <v>11</v>
-      </c>
-      <c r="T7" s="67">
-        <v>10</v>
-      </c>
-      <c r="U7" s="67">
-        <v>10</v>
-      </c>
-      <c r="V7" s="67">
-        <v>0</v>
-      </c>
-      <c r="W7" s="68">
-        <v>0.05</v>
-      </c>
-      <c r="X7" s="57">
-        <v>4.55</v>
-      </c>
+      <c r="S7" s="67"/>
+      <c r="T7" s="67"/>
+      <c r="U7" s="67"/>
+      <c r="V7" s="67"/>
+      <c r="W7" s="68"/>
+      <c r="X7" s="57"/>
     </row>
     <row r="8" spans="1:24" ht="95.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="13">
@@ -20706,24 +20658,12 @@
       <c r="R8" s="14">
         <v>7.22</v>
       </c>
-      <c r="S8" s="67">
-        <v>13</v>
-      </c>
-      <c r="T8" s="67">
-        <v>12</v>
-      </c>
-      <c r="U8" s="67">
-        <v>14</v>
-      </c>
-      <c r="V8" s="67">
-        <v>0</v>
-      </c>
-      <c r="W8" s="68">
-        <v>0.04</v>
-      </c>
-      <c r="X8" s="57">
-        <v>6.15</v>
-      </c>
+      <c r="S8" s="67"/>
+      <c r="T8" s="67"/>
+      <c r="U8" s="67"/>
+      <c r="V8" s="67"/>
+      <c r="W8" s="68"/>
+      <c r="X8" s="57"/>
     </row>
     <row r="9" spans="1:24" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A9" s="13">
@@ -20780,24 +20720,12 @@
       <c r="R9" s="14">
         <v>5.1100000000000003</v>
       </c>
-      <c r="S9" s="69">
-        <v>25</v>
-      </c>
-      <c r="T9" s="69">
-        <v>24</v>
-      </c>
-      <c r="U9" s="69">
-        <v>18</v>
-      </c>
-      <c r="V9" s="69">
-        <v>0</v>
-      </c>
-      <c r="W9" s="70">
-        <v>0.02</v>
-      </c>
-      <c r="X9" s="57">
-        <v>8.4</v>
-      </c>
+      <c r="S9" s="69"/>
+      <c r="T9" s="69"/>
+      <c r="U9" s="69"/>
+      <c r="V9" s="69"/>
+      <c r="W9" s="70"/>
+      <c r="X9" s="57"/>
     </row>
     <row r="10" spans="1:24" ht="40.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="13">
@@ -20854,24 +20782,12 @@
       <c r="R10" s="14">
         <v>7.86</v>
       </c>
-      <c r="S10" s="67">
-        <v>32</v>
-      </c>
-      <c r="T10" s="67">
-        <v>27</v>
-      </c>
-      <c r="U10" s="67">
-        <v>8</v>
-      </c>
-      <c r="V10" s="67">
-        <v>0</v>
-      </c>
-      <c r="W10" s="68">
-        <v>0.12</v>
-      </c>
-      <c r="X10" s="57">
-        <v>6.88</v>
-      </c>
+      <c r="S10" s="67"/>
+      <c r="T10" s="67"/>
+      <c r="U10" s="67"/>
+      <c r="V10" s="67"/>
+      <c r="W10" s="68"/>
+      <c r="X10" s="57"/>
     </row>
     <row r="11" spans="1:24" ht="55.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" s="13">
@@ -20928,24 +20844,12 @@
       <c r="R11" s="14">
         <v>6.88</v>
       </c>
-      <c r="S11" s="69">
-        <v>50</v>
-      </c>
-      <c r="T11" s="69">
-        <v>45</v>
-      </c>
-      <c r="U11" s="69">
-        <v>14</v>
-      </c>
-      <c r="V11" s="69">
-        <v>0</v>
-      </c>
-      <c r="W11" s="70">
-        <v>0.08</v>
-      </c>
-      <c r="X11" s="57">
-        <v>6.4</v>
-      </c>
+      <c r="S11" s="69"/>
+      <c r="T11" s="69"/>
+      <c r="U11" s="69"/>
+      <c r="V11" s="69"/>
+      <c r="W11" s="70"/>
+      <c r="X11" s="57"/>
     </row>
     <row r="12" spans="1:24" ht="48.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" s="13">
@@ -21002,24 +20906,12 @@
       <c r="R12" s="14">
         <v>4.74</v>
       </c>
-      <c r="S12" s="67">
-        <v>12</v>
-      </c>
-      <c r="T12" s="67">
-        <v>11</v>
-      </c>
-      <c r="U12" s="67">
-        <v>10</v>
-      </c>
-      <c r="V12" s="67">
-        <v>0</v>
-      </c>
-      <c r="W12" s="68">
-        <v>0.05</v>
-      </c>
-      <c r="X12" s="57">
-        <v>0</v>
-      </c>
+      <c r="S12" s="67"/>
+      <c r="T12" s="67"/>
+      <c r="U12" s="67"/>
+      <c r="V12" s="67"/>
+      <c r="W12" s="68"/>
+      <c r="X12" s="57"/>
     </row>
     <row r="13" spans="1:24" ht="71.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="13">
@@ -21076,24 +20968,12 @@
       <c r="R13" s="14">
         <v>2.86</v>
       </c>
-      <c r="S13" s="71">
-        <v>18</v>
-      </c>
-      <c r="T13" s="71">
-        <v>17</v>
-      </c>
-      <c r="U13" s="71">
-        <v>8</v>
-      </c>
-      <c r="V13" s="71">
-        <v>0</v>
-      </c>
-      <c r="W13" s="72">
-        <v>0.04</v>
-      </c>
-      <c r="X13" s="57">
-        <v>4.4400000000000004</v>
-      </c>
+      <c r="S13" s="71"/>
+      <c r="T13" s="71"/>
+      <c r="U13" s="71"/>
+      <c r="V13" s="71"/>
+      <c r="W13" s="72"/>
+      <c r="X13" s="57"/>
     </row>
     <row r="14" spans="1:24" ht="53.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="13">
@@ -21150,24 +21030,12 @@
       <c r="R14" s="14">
         <v>5.95</v>
       </c>
-      <c r="S14" s="73">
-        <v>22</v>
-      </c>
-      <c r="T14" s="73">
-        <v>20</v>
-      </c>
-      <c r="U14" s="73">
-        <v>10</v>
-      </c>
-      <c r="V14" s="73">
-        <v>0</v>
-      </c>
-      <c r="W14" s="74">
-        <v>0.06</v>
-      </c>
-      <c r="X14" s="57">
-        <v>6.96</v>
-      </c>
+      <c r="S14" s="73"/>
+      <c r="T14" s="73"/>
+      <c r="U14" s="73"/>
+      <c r="V14" s="73"/>
+      <c r="W14" s="74"/>
+      <c r="X14" s="57"/>
     </row>
     <row r="15" spans="1:24" ht="78.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="13">
@@ -21224,24 +21092,12 @@
       <c r="R15" s="14">
         <v>6.72</v>
       </c>
-      <c r="S15" s="71">
-        <v>37</v>
-      </c>
-      <c r="T15" s="71">
-        <v>32</v>
-      </c>
-      <c r="U15" s="71">
-        <v>16</v>
-      </c>
-      <c r="V15" s="71">
-        <v>0</v>
-      </c>
-      <c r="W15" s="72">
-        <v>0.09</v>
-      </c>
-      <c r="X15" s="57">
-        <v>8.92</v>
-      </c>
+      <c r="S15" s="71"/>
+      <c r="T15" s="71"/>
+      <c r="U15" s="71"/>
+      <c r="V15" s="71"/>
+      <c r="W15" s="72"/>
+      <c r="X15" s="57"/>
     </row>
     <row r="16" spans="1:24" ht="74.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="13">
@@ -21298,24 +21154,12 @@
       <c r="R16" s="14">
         <v>6.57</v>
       </c>
-      <c r="S16" s="73">
-        <v>34</v>
-      </c>
-      <c r="T16" s="73">
-        <v>30</v>
-      </c>
-      <c r="U16" s="73">
-        <v>10</v>
-      </c>
-      <c r="V16" s="73">
-        <v>0</v>
-      </c>
-      <c r="W16" s="74">
-        <v>0.09</v>
-      </c>
-      <c r="X16" s="57">
-        <v>6.47</v>
-      </c>
+      <c r="S16" s="73"/>
+      <c r="T16" s="73"/>
+      <c r="U16" s="73"/>
+      <c r="V16" s="73"/>
+      <c r="W16" s="74"/>
+      <c r="X16" s="57"/>
     </row>
     <row r="17" spans="1:24" ht="82.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="13">
@@ -21372,24 +21216,12 @@
       <c r="R17" s="14">
         <v>6.39</v>
       </c>
-      <c r="S17" s="71">
-        <v>13</v>
-      </c>
-      <c r="T17" s="71">
-        <v>12</v>
-      </c>
-      <c r="U17" s="71">
-        <v>8</v>
-      </c>
-      <c r="V17" s="71">
-        <v>0</v>
-      </c>
-      <c r="W17" s="72">
-        <v>0.05</v>
-      </c>
-      <c r="X17" s="57">
-        <v>6.15</v>
-      </c>
+      <c r="S17" s="71"/>
+      <c r="T17" s="71"/>
+      <c r="U17" s="71"/>
+      <c r="V17" s="71"/>
+      <c r="W17" s="72"/>
+      <c r="X17" s="57"/>
     </row>
     <row r="18" spans="1:24" ht="96" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="13">
@@ -21446,24 +21278,12 @@
       <c r="R18" s="14">
         <v>5.6</v>
       </c>
-      <c r="S18" s="73">
-        <v>28</v>
-      </c>
-      <c r="T18" s="73">
-        <v>27</v>
-      </c>
-      <c r="U18" s="73">
-        <v>23</v>
-      </c>
-      <c r="V18" s="73">
-        <v>0</v>
-      </c>
-      <c r="W18" s="74">
-        <v>0.02</v>
-      </c>
-      <c r="X18" s="57">
-        <v>6.43</v>
-      </c>
+      <c r="S18" s="73"/>
+      <c r="T18" s="73"/>
+      <c r="U18" s="73"/>
+      <c r="V18" s="73"/>
+      <c r="W18" s="74"/>
+      <c r="X18" s="57"/>
     </row>
     <row r="19" spans="1:24" ht="63" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="13">
@@ -21520,24 +21340,12 @@
       <c r="R19" s="14">
         <v>1.67</v>
       </c>
-      <c r="S19" s="71">
-        <v>6</v>
-      </c>
-      <c r="T19" s="71">
-        <v>5</v>
-      </c>
-      <c r="U19" s="71">
-        <v>4</v>
-      </c>
-      <c r="V19" s="71">
-        <v>0</v>
-      </c>
-      <c r="W19" s="72">
-        <v>0.1</v>
-      </c>
-      <c r="X19" s="57">
-        <v>0</v>
-      </c>
+      <c r="S19" s="71"/>
+      <c r="T19" s="71"/>
+      <c r="U19" s="71"/>
+      <c r="V19" s="71"/>
+      <c r="W19" s="72"/>
+      <c r="X19" s="57"/>
     </row>
     <row r="20" spans="1:24" ht="60.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="13">
@@ -21594,24 +21402,12 @@
       <c r="R20" s="14">
         <v>0.83</v>
       </c>
-      <c r="S20" s="73">
-        <v>9</v>
-      </c>
-      <c r="T20" s="73">
-        <v>7</v>
-      </c>
-      <c r="U20" s="73">
-        <v>2</v>
-      </c>
-      <c r="V20" s="73">
-        <v>0</v>
-      </c>
-      <c r="W20" s="74">
-        <v>0.18</v>
-      </c>
-      <c r="X20" s="57">
-        <v>3.33</v>
-      </c>
+      <c r="S20" s="73"/>
+      <c r="T20" s="73"/>
+      <c r="U20" s="73"/>
+      <c r="V20" s="73"/>
+      <c r="W20" s="74"/>
+      <c r="X20" s="57"/>
     </row>
     <row r="21" spans="1:24" ht="70.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="13">
@@ -21668,24 +21464,12 @@
       <c r="R21" s="14">
         <v>8.44</v>
       </c>
-      <c r="S21" s="71">
-        <v>14</v>
-      </c>
-      <c r="T21" s="71">
-        <v>13</v>
-      </c>
-      <c r="U21" s="71">
-        <v>12</v>
-      </c>
-      <c r="V21" s="71">
-        <v>0</v>
-      </c>
-      <c r="W21" s="72">
-        <v>0.04</v>
-      </c>
-      <c r="X21" s="57">
-        <v>3.57</v>
-      </c>
+      <c r="S21" s="71"/>
+      <c r="T21" s="71"/>
+      <c r="U21" s="71"/>
+      <c r="V21" s="71"/>
+      <c r="W21" s="72"/>
+      <c r="X21" s="57"/>
     </row>
     <row r="22" spans="1:24" ht="76.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="13">
@@ -21742,24 +21526,12 @@
       <c r="R22" s="14">
         <v>4.78</v>
       </c>
-      <c r="S22" s="73">
-        <v>8</v>
-      </c>
-      <c r="T22" s="73">
-        <v>7</v>
-      </c>
-      <c r="U22" s="73">
-        <v>4</v>
-      </c>
-      <c r="V22" s="73">
-        <v>0</v>
-      </c>
-      <c r="W22" s="74">
-        <v>0.08</v>
-      </c>
-      <c r="X22" s="57">
-        <v>0</v>
-      </c>
+      <c r="S22" s="73"/>
+      <c r="T22" s="73"/>
+      <c r="U22" s="73"/>
+      <c r="V22" s="73"/>
+      <c r="W22" s="74"/>
+      <c r="X22" s="57"/>
     </row>
     <row r="23" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A23" s="13">
@@ -21816,24 +21588,12 @@
       <c r="R23" s="14">
         <v>6.34</v>
       </c>
-      <c r="S23" s="67">
-        <v>27</v>
-      </c>
-      <c r="T23" s="67">
-        <v>25</v>
-      </c>
-      <c r="U23" s="67">
-        <v>18</v>
-      </c>
-      <c r="V23" s="67">
-        <v>0</v>
-      </c>
-      <c r="W23" s="68">
-        <v>0.04</v>
-      </c>
-      <c r="X23" s="57">
-        <v>6.67</v>
-      </c>
+      <c r="S23" s="67"/>
+      <c r="T23" s="67"/>
+      <c r="U23" s="67"/>
+      <c r="V23" s="67"/>
+      <c r="W23" s="68"/>
+      <c r="X23" s="57"/>
     </row>
     <row r="24" spans="1:24" ht="72" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A24" s="13">
@@ -21890,24 +21650,12 @@
       <c r="R24" s="14">
         <v>4.74</v>
       </c>
-      <c r="S24" s="69">
-        <v>13</v>
-      </c>
-      <c r="T24" s="69">
-        <v>12</v>
-      </c>
-      <c r="U24" s="69">
-        <v>8</v>
-      </c>
-      <c r="V24" s="69">
-        <v>0</v>
-      </c>
-      <c r="W24" s="70">
-        <v>0.05</v>
-      </c>
-      <c r="X24" s="57">
-        <v>3.85</v>
-      </c>
+      <c r="S24" s="69"/>
+      <c r="T24" s="69"/>
+      <c r="U24" s="69"/>
+      <c r="V24" s="69"/>
+      <c r="W24" s="70"/>
+      <c r="X24" s="57"/>
     </row>
     <row r="25" spans="1:24" ht="58.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A25" s="13">
@@ -21964,24 +21712,12 @@
       <c r="R25" s="14">
         <v>4.29</v>
       </c>
-      <c r="S25" s="67">
-        <v>16</v>
-      </c>
-      <c r="T25" s="67">
-        <v>15</v>
-      </c>
-      <c r="U25" s="67">
-        <v>10</v>
-      </c>
-      <c r="V25" s="67">
-        <v>0</v>
-      </c>
-      <c r="W25" s="68">
-        <v>0.04</v>
-      </c>
-      <c r="X25" s="57">
-        <v>3.12</v>
-      </c>
+      <c r="S25" s="67"/>
+      <c r="T25" s="67"/>
+      <c r="U25" s="67"/>
+      <c r="V25" s="67"/>
+      <c r="W25" s="68"/>
+      <c r="X25" s="57"/>
     </row>
     <row r="26" spans="1:24" ht="62.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A26" s="13">
@@ -22038,24 +21774,12 @@
       <c r="R26" s="14">
         <v>5.5</v>
       </c>
-      <c r="S26" s="69">
-        <v>16</v>
-      </c>
-      <c r="T26" s="69">
-        <v>14</v>
-      </c>
-      <c r="U26" s="69">
-        <v>2</v>
-      </c>
-      <c r="V26" s="69">
-        <v>0</v>
-      </c>
-      <c r="W26" s="70">
-        <v>0.11</v>
-      </c>
-      <c r="X26" s="57">
-        <v>4.38</v>
-      </c>
+      <c r="S26" s="69"/>
+      <c r="T26" s="69"/>
+      <c r="U26" s="69"/>
+      <c r="V26" s="69"/>
+      <c r="W26" s="70"/>
+      <c r="X26" s="57"/>
     </row>
     <row r="27" spans="1:24" ht="67.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A27" s="13">
@@ -22112,24 +21836,12 @@
       <c r="R27" s="14">
         <v>5.56</v>
       </c>
-      <c r="S27" s="67">
-        <v>9</v>
-      </c>
-      <c r="T27" s="67">
-        <v>8</v>
-      </c>
-      <c r="U27" s="67">
-        <v>4</v>
-      </c>
-      <c r="V27" s="67">
-        <v>0</v>
-      </c>
-      <c r="W27" s="68">
-        <v>0.08</v>
-      </c>
-      <c r="X27" s="57">
-        <v>2.2200000000000002</v>
-      </c>
+      <c r="S27" s="67"/>
+      <c r="T27" s="67"/>
+      <c r="U27" s="67"/>
+      <c r="V27" s="67"/>
+      <c r="W27" s="68"/>
+      <c r="X27" s="57"/>
     </row>
     <row r="28" spans="1:24" ht="65.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A28" s="13">
@@ -22186,24 +21898,12 @@
       <c r="R28" s="58">
         <v>4.4400000000000004</v>
       </c>
-      <c r="S28" s="69">
-        <v>29</v>
-      </c>
-      <c r="T28" s="69">
-        <v>28</v>
-      </c>
-      <c r="U28" s="69">
-        <v>8</v>
-      </c>
-      <c r="V28" s="69">
-        <v>0</v>
-      </c>
-      <c r="W28" s="70">
-        <v>0.03</v>
-      </c>
-      <c r="X28" s="57">
-        <v>7.59</v>
-      </c>
+      <c r="S28" s="69"/>
+      <c r="T28" s="69"/>
+      <c r="U28" s="69"/>
+      <c r="V28" s="69"/>
+      <c r="W28" s="70"/>
+      <c r="X28" s="57"/>
     </row>
     <row r="29" spans="1:24" ht="102" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A29" s="13">
@@ -22260,24 +21960,12 @@
       <c r="R29" s="58">
         <v>1.3</v>
       </c>
-      <c r="S29" s="67">
-        <v>23</v>
-      </c>
-      <c r="T29" s="67">
-        <v>22</v>
-      </c>
-      <c r="U29" s="67">
-        <v>18</v>
-      </c>
-      <c r="V29" s="67">
-        <v>0</v>
-      </c>
-      <c r="W29" s="68">
-        <v>0.02</v>
-      </c>
-      <c r="X29" s="57">
-        <v>4.78</v>
-      </c>
+      <c r="S29" s="67"/>
+      <c r="T29" s="67"/>
+      <c r="U29" s="67"/>
+      <c r="V29" s="67"/>
+      <c r="W29" s="68"/>
+      <c r="X29" s="57"/>
     </row>
     <row r="30" spans="1:24" ht="72.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A30" s="13">
@@ -22334,24 +22022,12 @@
       <c r="R30" s="58">
         <v>6.44</v>
       </c>
-      <c r="S30" s="69">
-        <v>14</v>
-      </c>
-      <c r="T30" s="69">
-        <v>13</v>
-      </c>
-      <c r="U30" s="69">
-        <v>10</v>
-      </c>
-      <c r="V30" s="69">
-        <v>0</v>
-      </c>
-      <c r="W30" s="70">
-        <v>0.04</v>
-      </c>
-      <c r="X30" s="57">
-        <v>4.29</v>
-      </c>
+      <c r="S30" s="69"/>
+      <c r="T30" s="69"/>
+      <c r="U30" s="69"/>
+      <c r="V30" s="69"/>
+      <c r="W30" s="70"/>
+      <c r="X30" s="57"/>
     </row>
     <row r="31" spans="1:24" ht="54.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A31" s="13">
@@ -22408,24 +22084,12 @@
       <c r="R31" s="58">
         <v>7.1</v>
       </c>
-      <c r="S31" s="67">
-        <v>13</v>
-      </c>
-      <c r="T31" s="67">
-        <v>12</v>
-      </c>
-      <c r="U31" s="67">
-        <v>12</v>
-      </c>
-      <c r="V31" s="67">
-        <v>0</v>
-      </c>
-      <c r="W31" s="68">
-        <v>0.04</v>
-      </c>
-      <c r="X31" s="57">
-        <v>5.38</v>
-      </c>
+      <c r="S31" s="67"/>
+      <c r="T31" s="67"/>
+      <c r="U31" s="67"/>
+      <c r="V31" s="67"/>
+      <c r="W31" s="68"/>
+      <c r="X31" s="57"/>
     </row>
     <row r="32" spans="1:24" ht="66.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A32" s="13">
@@ -22482,24 +22146,12 @@
       <c r="R32" s="58">
         <v>2.5</v>
       </c>
-      <c r="S32" s="69">
-        <v>7</v>
-      </c>
-      <c r="T32" s="69">
-        <v>6</v>
-      </c>
-      <c r="U32" s="69">
-        <v>6</v>
-      </c>
-      <c r="V32" s="69">
-        <v>0</v>
-      </c>
-      <c r="W32" s="70">
-        <v>0.08</v>
-      </c>
-      <c r="X32" s="57">
-        <v>2.86</v>
-      </c>
+      <c r="S32" s="69"/>
+      <c r="T32" s="69"/>
+      <c r="U32" s="69"/>
+      <c r="V32" s="69"/>
+      <c r="W32" s="70"/>
+      <c r="X32" s="57"/>
     </row>
     <row r="33" spans="1:24" ht="85.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A33" s="13">
@@ -22556,24 +22208,12 @@
       <c r="R33" s="58">
         <v>5.62</v>
       </c>
-      <c r="S33" s="75">
-        <v>18</v>
-      </c>
-      <c r="T33" s="75">
-        <v>17</v>
-      </c>
-      <c r="U33" s="75">
-        <v>12</v>
-      </c>
-      <c r="V33" s="75">
-        <v>0</v>
-      </c>
-      <c r="W33" s="76">
-        <v>0.03</v>
-      </c>
-      <c r="X33" s="57">
-        <v>7.22</v>
-      </c>
+      <c r="S33" s="75"/>
+      <c r="T33" s="75"/>
+      <c r="U33" s="75"/>
+      <c r="V33" s="75"/>
+      <c r="W33" s="76"/>
+      <c r="X33" s="57"/>
     </row>
     <row r="34" spans="1:24" ht="90" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A34" s="13">
@@ -22630,24 +22270,12 @@
       <c r="R34" s="58">
         <v>1.54</v>
       </c>
-      <c r="S34" s="77">
-        <v>19</v>
-      </c>
-      <c r="T34" s="77">
-        <v>17</v>
-      </c>
-      <c r="U34" s="77">
-        <v>12</v>
-      </c>
-      <c r="V34" s="77">
-        <v>0</v>
-      </c>
-      <c r="W34" s="78">
-        <v>0.06</v>
-      </c>
-      <c r="X34" s="57">
-        <v>3.16</v>
-      </c>
+      <c r="S34" s="77"/>
+      <c r="T34" s="77"/>
+      <c r="U34" s="77"/>
+      <c r="V34" s="77"/>
+      <c r="W34" s="78"/>
+      <c r="X34" s="57"/>
     </row>
     <row r="35" spans="1:24" ht="78" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A35" s="13">
@@ -22704,24 +22332,12 @@
       <c r="R35" s="58">
         <v>4</v>
       </c>
-      <c r="S35" s="75">
-        <v>32</v>
-      </c>
-      <c r="T35" s="75">
-        <v>29</v>
-      </c>
-      <c r="U35" s="75">
-        <v>22</v>
-      </c>
-      <c r="V35" s="75">
-        <v>0</v>
-      </c>
-      <c r="W35" s="76">
-        <v>0.06</v>
-      </c>
-      <c r="X35" s="57">
-        <v>4.0599999999999996</v>
-      </c>
+      <c r="S35" s="75"/>
+      <c r="T35" s="75"/>
+      <c r="U35" s="75"/>
+      <c r="V35" s="75"/>
+      <c r="W35" s="76"/>
+      <c r="X35" s="57"/>
     </row>
     <row r="36" spans="1:24" ht="82.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A36" s="13">
@@ -22778,24 +22394,12 @@
       <c r="R36" s="58">
         <v>6.9</v>
       </c>
-      <c r="S36" s="77">
-        <v>19</v>
-      </c>
-      <c r="T36" s="77">
-        <v>17</v>
-      </c>
-      <c r="U36" s="77">
-        <v>10</v>
-      </c>
-      <c r="V36" s="77">
-        <v>0</v>
-      </c>
-      <c r="W36" s="78">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="X36" s="57">
-        <v>6.32</v>
-      </c>
+      <c r="S36" s="77"/>
+      <c r="T36" s="77"/>
+      <c r="U36" s="77"/>
+      <c r="V36" s="77"/>
+      <c r="W36" s="78"/>
+      <c r="X36" s="57"/>
     </row>
     <row r="37" spans="1:24" ht="75.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A37" s="13">
@@ -22852,24 +22456,12 @@
       <c r="R37" s="58">
         <v>0</v>
       </c>
-      <c r="S37" s="75">
-        <v>20</v>
-      </c>
-      <c r="T37" s="75">
-        <v>19</v>
-      </c>
-      <c r="U37" s="75">
-        <v>8</v>
-      </c>
-      <c r="V37" s="75">
-        <v>0</v>
-      </c>
-      <c r="W37" s="76">
-        <v>0.04</v>
-      </c>
-      <c r="X37" s="57">
-        <v>2.5</v>
-      </c>
+      <c r="S37" s="75"/>
+      <c r="T37" s="75"/>
+      <c r="U37" s="75"/>
+      <c r="V37" s="75"/>
+      <c r="W37" s="76"/>
+      <c r="X37" s="57"/>
     </row>
     <row r="38" spans="1:24" ht="79.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A38" s="13">
@@ -22926,24 +22518,12 @@
       <c r="R38" s="58">
         <v>2</v>
       </c>
-      <c r="S38" s="77">
-        <v>19</v>
-      </c>
-      <c r="T38" s="77">
-        <v>17</v>
-      </c>
-      <c r="U38" s="77">
-        <v>14</v>
-      </c>
-      <c r="V38" s="77">
-        <v>0</v>
-      </c>
-      <c r="W38" s="78">
-        <v>0.06</v>
-      </c>
-      <c r="X38" s="57">
-        <v>5.26</v>
-      </c>
+      <c r="S38" s="77"/>
+      <c r="T38" s="77"/>
+      <c r="U38" s="77"/>
+      <c r="V38" s="77"/>
+      <c r="W38" s="78"/>
+      <c r="X38" s="57"/>
     </row>
     <row r="39" spans="1:24" ht="95.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A39" s="13">
@@ -23000,24 +22580,12 @@
       <c r="R39" s="58">
         <v>8.1199999999999992</v>
       </c>
-      <c r="S39" s="75">
-        <v>30</v>
-      </c>
-      <c r="T39" s="75">
-        <v>26</v>
-      </c>
-      <c r="U39" s="75">
-        <v>12</v>
-      </c>
-      <c r="V39" s="75">
-        <v>0</v>
-      </c>
-      <c r="W39" s="76">
-        <v>0.1</v>
-      </c>
-      <c r="X39" s="57">
-        <v>6.67</v>
-      </c>
+      <c r="S39" s="75"/>
+      <c r="T39" s="75"/>
+      <c r="U39" s="75"/>
+      <c r="V39" s="75"/>
+      <c r="W39" s="76"/>
+      <c r="X39" s="57"/>
     </row>
     <row r="40" spans="1:24" ht="86.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A40" s="13">
@@ -23074,24 +22642,12 @@
       <c r="R40" s="58">
         <v>1.54</v>
       </c>
-      <c r="S40" s="77">
-        <v>13</v>
-      </c>
-      <c r="T40" s="77">
-        <v>11</v>
-      </c>
-      <c r="U40" s="77">
-        <v>10</v>
-      </c>
-      <c r="V40" s="77">
-        <v>0</v>
-      </c>
-      <c r="W40" s="78">
-        <v>0.09</v>
-      </c>
-      <c r="X40" s="57">
-        <v>3.08</v>
-      </c>
+      <c r="S40" s="77"/>
+      <c r="T40" s="77"/>
+      <c r="U40" s="77"/>
+      <c r="V40" s="77"/>
+      <c r="W40" s="78"/>
+      <c r="X40" s="57"/>
     </row>
     <row r="41" spans="1:24" ht="70.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A41" s="13">
@@ -23148,24 +22704,12 @@
       <c r="R41" s="58">
         <v>5</v>
       </c>
-      <c r="S41" s="75">
-        <v>11</v>
-      </c>
-      <c r="T41" s="75">
-        <v>9</v>
-      </c>
-      <c r="U41" s="75">
-        <v>6</v>
-      </c>
-      <c r="V41" s="75">
-        <v>0</v>
-      </c>
-      <c r="W41" s="76">
-        <v>0.12</v>
-      </c>
-      <c r="X41" s="57">
-        <v>2.73</v>
-      </c>
+      <c r="S41" s="75"/>
+      <c r="T41" s="75"/>
+      <c r="U41" s="75"/>
+      <c r="V41" s="75"/>
+      <c r="W41" s="76"/>
+      <c r="X41" s="57"/>
     </row>
     <row r="42" spans="1:24" ht="85.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A42" s="13">
@@ -23222,24 +22766,12 @@
       <c r="R42" s="58">
         <v>1.74</v>
       </c>
-      <c r="S42" s="77">
-        <v>38</v>
-      </c>
-      <c r="T42" s="77">
-        <v>35</v>
-      </c>
-      <c r="U42" s="77">
-        <v>26</v>
-      </c>
-      <c r="V42" s="77">
-        <v>0</v>
-      </c>
-      <c r="W42" s="78">
-        <v>0.05</v>
-      </c>
-      <c r="X42" s="57">
-        <v>6.58</v>
-      </c>
+      <c r="S42" s="77"/>
+      <c r="T42" s="77"/>
+      <c r="U42" s="77"/>
+      <c r="V42" s="77"/>
+      <c r="W42" s="78"/>
+      <c r="X42" s="57"/>
     </row>
     <row r="43" spans="1:24" ht="84" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A43" s="13">
@@ -23296,24 +22828,12 @@
       <c r="R43" s="58">
         <v>7.81</v>
       </c>
-      <c r="S43" s="67">
-        <v>30</v>
-      </c>
-      <c r="T43" s="67">
-        <v>25</v>
-      </c>
-      <c r="U43" s="67">
-        <v>12</v>
-      </c>
-      <c r="V43" s="67">
-        <v>0</v>
-      </c>
-      <c r="W43" s="68">
-        <v>0.12</v>
-      </c>
-      <c r="X43" s="57">
-        <v>6</v>
-      </c>
+      <c r="S43" s="67"/>
+      <c r="T43" s="67"/>
+      <c r="U43" s="67"/>
+      <c r="V43" s="67"/>
+      <c r="W43" s="68"/>
+      <c r="X43" s="57"/>
     </row>
     <row r="44" spans="1:24" ht="85.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A44" s="13">
@@ -23370,24 +22890,12 @@
       <c r="R44" s="58">
         <v>4.78</v>
       </c>
-      <c r="S44" s="69">
-        <v>10</v>
-      </c>
-      <c r="T44" s="69">
-        <v>9</v>
-      </c>
-      <c r="U44" s="69">
-        <v>8</v>
-      </c>
-      <c r="V44" s="69">
-        <v>0</v>
-      </c>
-      <c r="W44" s="70">
-        <v>0.06</v>
-      </c>
-      <c r="X44" s="57">
-        <v>4</v>
-      </c>
+      <c r="S44" s="69"/>
+      <c r="T44" s="69"/>
+      <c r="U44" s="69"/>
+      <c r="V44" s="69"/>
+      <c r="W44" s="70"/>
+      <c r="X44" s="57"/>
     </row>
     <row r="45" spans="1:24" ht="94.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A45" s="13">
@@ -23444,24 +22952,12 @@
       <c r="R45" s="58">
         <v>6.76</v>
       </c>
-      <c r="S45" s="67">
-        <v>18</v>
-      </c>
-      <c r="T45" s="67">
-        <v>17</v>
-      </c>
-      <c r="U45" s="67">
-        <v>16</v>
-      </c>
-      <c r="V45" s="67">
-        <v>0</v>
-      </c>
-      <c r="W45" s="68">
-        <v>0.03</v>
-      </c>
-      <c r="X45" s="57">
-        <v>3.89</v>
-      </c>
+      <c r="S45" s="67"/>
+      <c r="T45" s="67"/>
+      <c r="U45" s="67"/>
+      <c r="V45" s="67"/>
+      <c r="W45" s="68"/>
+      <c r="X45" s="57"/>
     </row>
     <row r="46" spans="1:24" ht="117.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A46" s="13">
@@ -23518,24 +23014,12 @@
       <c r="R46" s="58">
         <v>5.43</v>
       </c>
-      <c r="S46" s="69">
-        <v>9</v>
-      </c>
-      <c r="T46" s="69">
-        <v>7</v>
-      </c>
-      <c r="U46" s="69">
-        <v>6</v>
-      </c>
-      <c r="V46" s="69">
-        <v>0</v>
-      </c>
-      <c r="W46" s="70">
-        <v>0.13</v>
-      </c>
-      <c r="X46" s="57">
-        <v>0</v>
-      </c>
+      <c r="S46" s="69"/>
+      <c r="T46" s="69"/>
+      <c r="U46" s="69"/>
+      <c r="V46" s="69"/>
+      <c r="W46" s="70"/>
+      <c r="X46" s="57"/>
     </row>
     <row r="47" spans="1:24" ht="98.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A47" s="13">
@@ -23592,24 +23076,12 @@
       <c r="R47" s="58">
         <v>3.33</v>
       </c>
-      <c r="S47" s="67">
-        <v>12</v>
-      </c>
-      <c r="T47" s="67">
-        <v>10</v>
-      </c>
-      <c r="U47" s="67">
-        <v>10</v>
-      </c>
-      <c r="V47" s="67">
-        <v>0</v>
-      </c>
-      <c r="W47" s="68">
-        <v>0.09</v>
-      </c>
-      <c r="X47" s="57">
-        <v>2.5</v>
-      </c>
+      <c r="S47" s="67"/>
+      <c r="T47" s="67"/>
+      <c r="U47" s="67"/>
+      <c r="V47" s="67"/>
+      <c r="W47" s="68"/>
+      <c r="X47" s="57"/>
     </row>
     <row r="48" spans="1:24" ht="89.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A48" s="13">
@@ -23666,24 +23138,12 @@
       <c r="R48" s="58">
         <v>0.77</v>
       </c>
-      <c r="S48" s="69">
-        <v>16</v>
-      </c>
-      <c r="T48" s="69">
-        <v>13</v>
-      </c>
-      <c r="U48" s="69">
-        <v>6</v>
-      </c>
-      <c r="V48" s="69">
-        <v>0</v>
-      </c>
-      <c r="W48" s="70">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="X48" s="57">
-        <v>3.75</v>
-      </c>
+      <c r="S48" s="69"/>
+      <c r="T48" s="69"/>
+      <c r="U48" s="69"/>
+      <c r="V48" s="69"/>
+      <c r="W48" s="70"/>
+      <c r="X48" s="57"/>
     </row>
     <row r="49" spans="1:24" ht="80.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A49" s="13">
@@ -23740,24 +23200,12 @@
       <c r="R49" s="58">
         <v>5.56</v>
       </c>
-      <c r="S49" s="67">
-        <v>11</v>
-      </c>
-      <c r="T49" s="67">
-        <v>9</v>
-      </c>
-      <c r="U49" s="67">
-        <v>6</v>
-      </c>
-      <c r="V49" s="67">
-        <v>0</v>
-      </c>
-      <c r="W49" s="68">
-        <v>0.12</v>
-      </c>
-      <c r="X49" s="57">
-        <v>3.64</v>
-      </c>
+      <c r="S49" s="67"/>
+      <c r="T49" s="67"/>
+      <c r="U49" s="67"/>
+      <c r="V49" s="67"/>
+      <c r="W49" s="68"/>
+      <c r="X49" s="57"/>
     </row>
     <row r="50" spans="1:24" ht="69" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A50" s="13">
@@ -23814,24 +23262,12 @@
       <c r="R50" s="58">
         <v>5.67</v>
       </c>
-      <c r="S50" s="69">
-        <v>12</v>
-      </c>
-      <c r="T50" s="69">
-        <v>10</v>
-      </c>
-      <c r="U50" s="69">
-        <v>10</v>
-      </c>
-      <c r="V50" s="69">
-        <v>0</v>
-      </c>
-      <c r="W50" s="70">
-        <v>0.09</v>
-      </c>
-      <c r="X50" s="57">
-        <v>2.5</v>
-      </c>
+      <c r="S50" s="69"/>
+      <c r="T50" s="69"/>
+      <c r="U50" s="69"/>
+      <c r="V50" s="69"/>
+      <c r="W50" s="70"/>
+      <c r="X50" s="57"/>
     </row>
     <row r="51" spans="1:24" ht="109.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A51" s="13">
@@ -23888,24 +23324,12 @@
       <c r="R51" s="58">
         <v>2.31</v>
       </c>
-      <c r="S51" s="67">
-        <v>10</v>
-      </c>
-      <c r="T51" s="67">
-        <v>9</v>
-      </c>
-      <c r="U51" s="67">
-        <v>6</v>
-      </c>
-      <c r="V51" s="67">
-        <v>0</v>
-      </c>
-      <c r="W51" s="68">
-        <v>0.06</v>
-      </c>
-      <c r="X51" s="57">
-        <v>2</v>
-      </c>
+      <c r="S51" s="67"/>
+      <c r="T51" s="67"/>
+      <c r="U51" s="67"/>
+      <c r="V51" s="67"/>
+      <c r="W51" s="68"/>
+      <c r="X51" s="57"/>
     </row>
     <row r="52" spans="1:24" ht="88.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A52" s="13">
@@ -23962,24 +23386,12 @@
       <c r="R52" s="58">
         <v>5.16</v>
       </c>
-      <c r="S52" s="69">
-        <v>26</v>
-      </c>
-      <c r="T52" s="69">
-        <v>24</v>
-      </c>
-      <c r="U52" s="69">
-        <v>8</v>
-      </c>
-      <c r="V52" s="69">
-        <v>0</v>
-      </c>
-      <c r="W52" s="70">
-        <v>0.06</v>
-      </c>
-      <c r="X52" s="57">
-        <v>3.85</v>
-      </c>
+      <c r="S52" s="69"/>
+      <c r="T52" s="69"/>
+      <c r="U52" s="69"/>
+      <c r="V52" s="69"/>
+      <c r="W52" s="70"/>
+      <c r="X52" s="57"/>
     </row>
     <row r="53" spans="1:24" ht="139.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A53" s="13">
@@ -24036,24 +23448,12 @@
       <c r="R53" s="58">
         <v>2.5</v>
       </c>
-      <c r="S53" s="69">
-        <v>12</v>
-      </c>
-      <c r="T53" s="69">
-        <v>10</v>
-      </c>
-      <c r="U53" s="69">
-        <v>12</v>
-      </c>
-      <c r="V53" s="69">
-        <v>0</v>
-      </c>
-      <c r="W53" s="70">
-        <v>0.08</v>
-      </c>
-      <c r="X53" s="57">
-        <v>3.33</v>
-      </c>
+      <c r="S53" s="69"/>
+      <c r="T53" s="69"/>
+      <c r="U53" s="69"/>
+      <c r="V53" s="69"/>
+      <c r="W53" s="70"/>
+      <c r="X53" s="57"/>
     </row>
     <row r="54" spans="1:24" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A54" s="13"/>
@@ -24124,13 +23524,13 @@
       <c r="T55" s="59"/>
       <c r="U55" s="59"/>
       <c r="V55" s="59"/>
-      <c r="W55" s="59">
+      <c r="W55" s="59" t="e">
         <f>AVERAGE(W4:W53)</f>
-        <v>0.10519999999999996</v>
-      </c>
-      <c r="X55" s="33">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X55" s="33" t="e">
         <f>AVERAGE(X4:X53)</f>
-        <v>4.3371999999999993</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="56" spans="1:24" ht="63" x14ac:dyDescent="0.5">
@@ -24176,13 +23576,13 @@
       <c r="T56" s="59"/>
       <c r="U56" s="59"/>
       <c r="V56" s="59"/>
-      <c r="W56" s="59">
+      <c r="W56" s="59" t="e">
         <f>STDEV(W4:W53)</f>
-        <v>0.17789288223821786</v>
-      </c>
-      <c r="X56" s="33">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X56" s="33" t="e">
         <f>STDEV(X4:X53)</f>
-        <v>2.1926863963305521</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="57" spans="1:24" ht="33.75" x14ac:dyDescent="0.5">

</xml_diff>